<commit_message>
capmin.plot now plots demand or caps; moosh/data.xlsx forces Elec only solution
</commit_message>
<xml_diff>
--- a/data/moosh/data.xlsx
+++ b/data/moosh/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="4"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -1240,11 +1240,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1296,7 @@
         <v>1E-3</v>
       </c>
       <c r="E2" s="6">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="F2" s="10">
         <v>0.01</v>
@@ -1322,7 +1322,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="E3" s="6">
-        <v>0.6</v>
+        <v>0.35</v>
       </c>
       <c r="F3" s="10">
         <v>1E-3</v>
@@ -1464,7 +1464,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -2133,11 +2133,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2237,10 +2237,10 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,7 +2269,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="27">
-        <v>0.95</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated runmoosh.py and data.xlsx with devs from haag_wgs84
</commit_message>
<xml_diff>
--- a/data/moosh/data.xlsx
+++ b/data/moosh/data.xlsx
@@ -1299,13 +1299,13 @@
         <v>0.3</v>
       </c>
       <c r="F2" s="10">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="G2" s="10">
         <v>0</v>
       </c>
       <c r="H2" s="3">
-        <v>2500000</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1325,13 +1325,13 @@
         <v>0.35</v>
       </c>
       <c r="F3" s="10">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="G3" s="10">
         <v>0</v>
       </c>
       <c r="H3" s="3">
-        <v>5000000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1342,16 +1342,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="3">
-        <v>200</v>
+        <v>1500</v>
       </c>
       <c r="D4" s="3">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E4" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F4" s="10">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G4" s="10">
         <v>2.0000000000000002E-5</v>
@@ -1368,16 +1368,16 @@
         <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>200</v>
+        <v>1500</v>
       </c>
       <c r="D5" s="3">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E5" s="6">
         <v>0.08</v>
       </c>
       <c r="F5" s="10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G5" s="10">
         <v>1.6000000000000001E-4</v>
@@ -1464,7 +1464,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,7 +1507,7 @@
         <v>10000</v>
       </c>
       <c r="C2" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -1562,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="35">
-        <v>44000</v>
+        <v>1000</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>61</v>
@@ -1631,7 +1631,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="35">
-        <v>99999</v>
+        <v>999990</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>64</v>
@@ -1645,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1654,7 +1654,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="35">
-        <v>55000</v>
+        <v>1000</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>66</v>
@@ -1704,7 +1704,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,7 +1894,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="8">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>